<commit_message>
Implement patient discharge and change treatment logic.
A public static final Stage object (Stage.Complete) was created to
provide a single stage object that is returned by the StageManager when
a patient has completed all of their stages, signified by a treatment ID
of 0 in the trajectories list of the setup.xlsx file.

Simulation logic was updated to check if a patient is in the Complete
stage, and discharges the patient from the hospital if so by removing
them from the current patient list.

The treatment logic in TreatmentPlan was updated so that the new
probability of mortality for a given condition after treatment follows a
geometric decay that is independent of the current treatment cycle.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="3820" windowWidth="18300" windowHeight="12860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="260" yWindow="680" windowWidth="28920" windowHeight="12860" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -94,9 +94,6 @@
     <t>0-1</t>
   </si>
   <si>
-    <t>0.05,0.05</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>48</t>
   </si>
   <si>
-    <t>0.05</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -304,9 +298,6 @@
     <t>50,125</t>
   </si>
   <si>
-    <t>0.05,0.1</t>
-  </si>
-  <si>
     <t>ECLAMPSIA</t>
   </si>
   <si>
@@ -343,13 +334,16 @@
     <t>MISOPROSTOL,MG_SO4,HYDRALAZINE,DEXAMETHASONE</t>
   </si>
   <si>
-    <t>0.05,05</t>
-  </si>
-  <si>
-    <t>Mean POM</t>
-  </si>
-  <si>
-    <t>Std POM</t>
+    <t>POM Mean</t>
+  </si>
+  <si>
+    <t>POM Stdev</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.2,0.2</t>
   </si>
 </sst>
 </file>
@@ -704,7 +698,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,16 +710,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,7 +752,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>0.19</v>
@@ -786,7 +780,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>0.55000000000000004</v>
@@ -807,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,10 +812,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -843,7 +837,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>8.6E-3</v>
@@ -859,7 +853,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6">
         <v>8.9999999999999998E-4</v>
@@ -874,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -960,13 +954,13 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -975,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -990,15 +984,15 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1010,13 +1004,13 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -1028,27 +1022,27 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
@@ -1060,13 +1054,13 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1075,10 +1069,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
@@ -1090,15 +1084,15 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -1110,13 +1104,13 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1128,27 +1122,27 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -1160,13 +1154,13 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1178,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
@@ -1190,15 +1184,15 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
@@ -1210,13 +1204,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -1228,645 +1222,645 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="P7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1878,45 +1872,45 @@
         <v>1</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1928,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
@@ -1940,33 +1934,33 @@
         <v>0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1978,622 +1972,622 @@
         <v>1</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="P22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="P32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify bug in model and add additional outputs.
Added number of patients and number of deaths per cycle to the model
output.

Fixed bug with probability of mortality for a given cycle, where the
cycle POM was going to unity when there were 0 remaining cycles left in
the patient's stay.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="680" windowWidth="28920" windowHeight="12860" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4420" yWindow="2320" windowWidth="28920" windowHeight="17840" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="2" r:id="rId1"/>
     <sheet name="Incidences" sheetId="3" r:id="rId2"/>
     <sheet name="Trajectories" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1610,7 +1610,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>66</v>
@@ -1737,7 +1737,7 @@
         <v>26</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Update trajectories and set oxytocin stock to 15,000U.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/M3/Dropbox/Development/BU/MMHModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34e1bedcffeeb701/Documents/Global Health Technologies Program/Modeling/MMH Model/Code/MMHModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="2320" windowWidth="28920" windowHeight="17840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="2910" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="2" r:id="rId1"/>
@@ -21,15 +21,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -226,24 +223,15 @@
     <t>OXYTOCIN,LIGNOCAINE</t>
   </si>
   <si>
-    <t>PARACETAMOL,DICLOFENAC,TRAMADOL</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
     <t>40,10</t>
   </si>
   <si>
-    <t>125,125,125</t>
-  </si>
-  <si>
     <t>0,0</t>
   </si>
   <si>
-    <t>0,0,0</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -286,9 +274,6 @@
     <t>DELIVERY,RU</t>
   </si>
   <si>
-    <t>OXYTOCIN,ERYTHROMYCIN</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -343,10 +328,43 @@
     <t>0.2,0.2</t>
   </si>
   <si>
-    <t>ERYTHROMYCIN,PARACETAMOL,DICLOFENAC_NA_LIQ</t>
-  </si>
-  <si>
-    <t>PARACETAMOL,DICLOFENAC_NA_LIQ,TRAMADOL</t>
+    <t>1000,50,500,1,</t>
+  </si>
+  <si>
+    <t>PARACETAMOL,DICLOFENAC_NA_LIQ,METRONIDAZOLE_LIQ,CEFTRIAXONE</t>
+  </si>
+  <si>
+    <t>32,32,32,0</t>
+  </si>
+  <si>
+    <t>DELIVERY,SEPSIS</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>METRONIDAZOLE_LIQ,CEFTRIAXONE</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>500,1</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>SEPSIS</t>
   </si>
 </sst>
 </file>
@@ -698,34 +716,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -739,7 +757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -753,9 +771,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>0.19</v>
@@ -767,7 +785,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -781,9 +799,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>0.55000000000000004</v>
@@ -793,6 +811,20 @@
       </c>
       <c r="D6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -802,15 +834,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,16 +853,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2">
         <f>1-SUM(B3:B1048576)</f>
-        <v>0.95050000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.94550000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -838,15 +870,15 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -854,12 +886,20 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -869,28 +909,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="31.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.875" style="1"/>
     <col min="9" max="9" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -959,8 +999,8 @@
       <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
@@ -993,7 +1033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1010,7 +1050,7 @@
         <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>45</v>
@@ -1060,7 +1100,7 @@
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>35</v>
@@ -1251,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -1260,13 +1300,13 @@
         <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>42</v>
@@ -1301,16 +1341,16 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>51</v>
@@ -1351,7 +1391,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -1360,7 +1400,7 @@
         <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>35</v>
@@ -1401,7 +1441,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -1410,7 +1450,7 @@
         <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>57</v>
@@ -1451,7 +1491,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
@@ -1460,7 +1500,7 @@
         <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>60</v>
@@ -1501,7 +1541,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -1510,7 +1550,7 @@
         <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>60</v>
@@ -1551,7 +1591,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -1560,7 +1600,7 @@
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>35</v>
@@ -1590,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1601,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -1610,10 +1650,10 @@
         <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>26</v>
@@ -1640,7 +1680,7 @@
         <v>28</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1651,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -1660,13 +1700,13 @@
         <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>28</v>
@@ -1690,7 +1730,7 @@
         <v>42</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1701,7 +1741,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -1710,10 +1750,10 @@
         <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>26</v>
@@ -1737,10 +1777,10 @@
         <v>26</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1751,7 +1791,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -1760,7 +1800,7 @@
         <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>26</v>
@@ -1801,22 +1841,22 @@
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>42</v>
@@ -1845,13 +1885,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -1860,7 +1900,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>26</v>
@@ -1890,18 +1930,18 @@
         <v>41</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
@@ -1910,7 +1950,7 @@
         <v>43</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>26</v>
@@ -1940,18 +1980,18 @@
         <v>48</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
@@ -1960,7 +2000,7 @@
         <v>43</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>26</v>
@@ -1995,28 +2035,28 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
@@ -2040,27 +2080,27 @@
         <v>28</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>51</v>
@@ -2090,27 +2130,27 @@
         <v>46</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>35</v>
@@ -2140,27 +2180,27 @@
         <v>30</v>
       </c>
       <c r="P25" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>57</v>
@@ -2190,27 +2230,27 @@
         <v>54</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>60</v>
@@ -2240,27 +2280,27 @@
         <v>55</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>60</v>
@@ -2293,24 +2333,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>26</v>
@@ -2340,33 +2380,33 @@
         <v>28</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>29</v>
@@ -2390,33 +2430,33 @@
         <v>32</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>42</v>
@@ -2443,24 +2483,24 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>26</v>
@@ -2493,24 +2533,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>26</v>
@@ -2540,33 +2580,33 @@
         <v>32</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>42</v>
@@ -2590,6 +2630,256 @@
         <v>55</v>
       </c>
       <c r="P34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P39" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved variable for new patient probability to Hospital class
Created Hospital.setNewPatientProbability(double newPatientProbability)

Added Simulator.timeCheck()

Updated setup file
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -181,9 +181,6 @@
     <t>95</t>
   </si>
   <si>
-    <t>50,5,5,12</t>
-  </si>
-  <si>
     <t>MG_SO4,HYDRALAZINE</t>
   </si>
   <si>
@@ -316,12 +313,6 @@
     <t>POM Stdev</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.2,0.2</t>
-  </si>
-  <si>
     <t>32,32,32,0</t>
   </si>
   <si>
@@ -409,10 +400,28 @@
     <t>52</t>
   </si>
   <si>
-    <t>0.5,0.5</t>
-  </si>
-  <si>
     <t>32,32,0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.1,0.139</t>
+  </si>
+  <si>
+    <t>0.1,0.108</t>
+  </si>
+  <si>
+    <t>0.1,0.136</t>
+  </si>
+  <si>
+    <t>0.1,0.107</t>
+  </si>
+  <si>
+    <t>0.1,0.104</t>
+  </si>
+  <si>
+    <t>50,5,5,1</t>
   </si>
 </sst>
 </file>
@@ -473,7 +482,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -481,7 +490,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -766,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,10 +790,10 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -799,10 +807,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <f>0.01*B2</f>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="D2">
-        <v>1000000000</v>
+        <v>7796</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,24 +822,26 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <f t="shared" ref="C3:C7" si="0">0.01*B3</f>
+        <v>3.8000000000000002E-4</v>
       </c>
       <c r="D3" s="4">
-        <v>10000</v>
+        <v>9190</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="C4">
-        <v>0.25</v>
+        <f t="shared" si="0"/>
+        <v>3.5999999999999997E-4</v>
       </c>
       <c r="D4">
-        <v>5000</v>
+        <v>21847</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,38 +852,41 @@
         <v>0.11</v>
       </c>
       <c r="C5">
-        <v>0.35</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6">
         <v>0.27300000000000002</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.2</v>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2.7300000000000002E-3</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C7" s="5">
-        <v>0.17</v>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000001E-4</v>
       </c>
       <c r="D7">
-        <v>10000</v>
+        <v>8568</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +935,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>8.6E-3</v>
@@ -937,7 +951,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6">
         <v>8.9999999999999998E-4</v>
@@ -945,7 +959,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>5.0000000000000001E-3</v>
@@ -960,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1054,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1090,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -1099,7 +1113,7 @@
         <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>44</v>
@@ -1126,7 +1140,7 @@
         <v>32</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>28</v>
@@ -1140,7 +1154,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -1149,7 +1163,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>34</v>
@@ -1190,7 +1204,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
@@ -1240,7 +1254,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
@@ -1290,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
@@ -1340,7 +1354,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -1349,7 +1363,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>44</v>
@@ -1376,7 +1390,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>26</v>
@@ -1390,7 +1404,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
@@ -1399,7 +1413,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>34</v>
@@ -1440,7 +1454,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
@@ -1490,7 +1504,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
@@ -1540,7 +1554,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
@@ -1590,22 +1604,22 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>41</v>
@@ -1640,22 +1654,22 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>41</v>
@@ -1690,7 +1704,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
@@ -1699,7 +1713,7 @@
         <v>43</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>34</v>
@@ -1740,22 +1754,22 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>41</v>
@@ -1776,7 +1790,7 @@
         <v>39</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>40</v>
@@ -1790,22 +1804,22 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>41</v>
@@ -1826,7 +1840,7 @@
         <v>46</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>25</v>
@@ -1834,28 +1848,28 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>41</v>
@@ -1879,33 +1893,33 @@
         <v>27</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>41</v>
@@ -1929,18 +1943,18 @@
         <v>45</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>16</v>
@@ -1949,7 +1963,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>34</v>
@@ -1979,33 +1993,33 @@
         <v>29</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>41</v>
@@ -2026,36 +2040,36 @@
         <v>39</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>41</v>
@@ -2076,7 +2090,7 @@
         <v>46</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>25</v>
@@ -2084,28 +2098,28 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>41</v>
@@ -2129,33 +2143,33 @@
         <v>27</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>41</v>
@@ -2179,18 +2193,18 @@
         <v>45</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>16</v>
@@ -2199,7 +2213,7 @@
         <v>43</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>34</v>
@@ -2229,33 +2243,33 @@
         <v>29</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>41</v>
@@ -2276,36 +2290,36 @@
         <v>39</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>41</v>
@@ -2334,13 +2348,13 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>19</v>
@@ -2379,18 +2393,18 @@
         <v>29</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>19</v>
@@ -2399,10 +2413,10 @@
         <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>25</v>
@@ -2429,18 +2443,18 @@
         <v>27</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>19</v>
@@ -2452,10 +2466,10 @@
         <v>126</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>27</v>
@@ -2479,18 +2493,18 @@
         <v>41</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>19</v>
@@ -2502,7 +2516,7 @@
         <v>126</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>25</v>
@@ -2540,7 +2554,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
@@ -2549,7 +2563,7 @@
         <v>42</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>25</v>
@@ -2579,33 +2593,33 @@
         <v>31</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>126</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>41</v>
@@ -2626,7 +2640,7 @@
         <v>25</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>25</v>
@@ -2634,13 +2648,13 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>19</v>
@@ -2649,7 +2663,7 @@
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>25</v>
@@ -2679,18 +2693,18 @@
         <v>40</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>19</v>
@@ -2699,7 +2713,7 @@
         <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>25</v>
@@ -2729,18 +2743,18 @@
         <v>47</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>19</v>
@@ -2749,7 +2763,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>25</v>
@@ -2784,28 +2798,28 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>41</v>
@@ -2829,33 +2843,33 @@
         <v>27</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>41</v>
@@ -2879,27 +2893,27 @@
         <v>45</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>34</v>
@@ -2929,33 +2943,33 @@
         <v>29</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>41</v>
@@ -2976,36 +2990,36 @@
         <v>39</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>41</v>
@@ -3026,36 +3040,36 @@
         <v>46</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>41</v>
@@ -3076,7 +3090,7 @@
         <v>49</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>25</v>
@@ -3084,22 +3098,22 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>25</v>
@@ -3129,33 +3143,33 @@
         <v>27</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>28</v>
@@ -3179,33 +3193,33 @@
         <v>31</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H45" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>41</v>
@@ -3226,30 +3240,30 @@
         <v>25</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>25</v>
@@ -3284,22 +3298,22 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>25</v>
@@ -3329,33 +3343,33 @@
         <v>31</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H48" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>41</v>
@@ -3376,7 +3390,7 @@
         <v>25</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>45</v>
@@ -3387,25 +3401,25 @@
         <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>41</v>
@@ -3429,33 +3443,33 @@
         <v>27</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>41</v>
@@ -3476,7 +3490,7 @@
         <v>46</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>25</v>
@@ -3484,28 +3498,28 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>41</v>
@@ -3529,33 +3543,33 @@
         <v>27</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>28</v>
@@ -3579,33 +3593,33 @@
         <v>31</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H53" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>41</v>
@@ -3626,7 +3640,7 @@
         <v>25</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>25</v>

</xml_diff>